<commit_message>
Mettre done les taches effectuées dans le backlog
</commit_message>
<xml_diff>
--- a/BackLog.xlsx
+++ b/BackLog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Android\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\533\Desktop\ProjetAndroidGestionTaches\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -205,7 +205,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,6 +236,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -369,7 +375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -398,6 +404,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,24 +415,6 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
         <right/>
         <top style="thin">
           <color indexed="64"/>
@@ -535,6 +524,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
@@ -549,12 +554,14 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
   </dxfs>
@@ -571,7 +578,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:E40" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:E40" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
   <autoFilter ref="A1:E40">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -580,11 +587,11 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" name="ID" dataDxfId="5"/>
-    <tableColumn id="2" name="Critère" dataDxfId="4"/>
-    <tableColumn id="3" name="Estimation Effort" dataDxfId="3"/>
-    <tableColumn id="4" name="Ordre" dataDxfId="2"/>
-    <tableColumn id="5" name="Description" dataDxfId="1"/>
+    <tableColumn id="1" name="ID" dataDxfId="4"/>
+    <tableColumn id="2" name="Critère" dataDxfId="3"/>
+    <tableColumn id="3" name="Estimation Effort" dataDxfId="2"/>
+    <tableColumn id="4" name="Ordre" dataDxfId="1"/>
+    <tableColumn id="5" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -865,7 +872,7 @@
     <col min="5" max="5" width="107.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1353,10 +1360,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1364,7 +1371,7 @@
     <col min="5" max="5" width="89.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>48</v>
       </c>
@@ -1373,7 +1380,7 @@
       <c r="D1" s="21"/>
       <c r="E1" s="21"/>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
@@ -1390,7 +1397,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -1405,7 +1412,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="12" t="s">
         <v>6</v>
@@ -1415,8 +1422,9 @@
       <c r="E4" s="12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="22"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="12" t="s">
         <v>7</v>
@@ -1426,8 +1434,9 @@
       <c r="E5" s="12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="22"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="12" t="s">
         <v>9</v>
@@ -1438,7 +1447,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>2</v>
       </c>
@@ -1452,8 +1461,9 @@
       <c r="E7" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="22"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="12" t="s">
         <v>6</v>
@@ -1463,8 +1473,9 @@
       <c r="E8" s="12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="22"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="12" t="s">
         <v>7</v>
@@ -1474,8 +1485,9 @@
       <c r="E9" s="12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="22"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>3</v>
       </c>
@@ -1490,7 +1502,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="12" t="s">
         <v>6</v>
@@ -1501,7 +1513,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="12" t="s">
         <v>7</v>
@@ -1512,7 +1524,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="12" t="s">
         <v>9</v>
@@ -1523,7 +1535,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="12" t="s">
         <v>21</v>
@@ -1534,7 +1546,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="12" t="s">
         <v>22</v>
@@ -1545,7 +1557,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="12" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Ajout de user dans BD lors du signup
</commit_message>
<xml_diff>
--- a/BackLog.xlsx
+++ b/BackLog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\533\Desktop\ProjetAndroidGestionTaches\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\533\Documents\ProjetAndroidGestionTaches\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -401,10 +401,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -862,7 +862,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
@@ -1363,7 +1363,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1372,13 +1372,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1411,6 +1411,7 @@
       <c r="E3" s="8" t="s">
         <v>5</v>
       </c>
+      <c r="F3" s="21"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
@@ -1422,7 +1423,7 @@
       <c r="E4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="22"/>
+      <c r="F4" s="21"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
@@ -1434,7 +1435,7 @@
       <c r="E5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="22"/>
+      <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
@@ -1446,6 +1447,7 @@
       <c r="E6" s="12" t="s">
         <v>10</v>
       </c>
+      <c r="F6" s="21"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
@@ -1461,7 +1463,7 @@
       <c r="E7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="22"/>
+      <c r="F7" s="21"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
@@ -1473,7 +1475,7 @@
       <c r="E8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="22"/>
+      <c r="F8" s="21"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
@@ -1485,7 +1487,7 @@
       <c r="E9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="22"/>
+      <c r="F9" s="21"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8">

</xml_diff>